<commit_message>
MASTER: Add new mdc results.
</commit_message>
<xml_diff>
--- a/doc/mdc.xlsx
+++ b/doc/mdc.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="54">
   <si>
     <t>Normalization function</t>
   </si>
@@ -30,6 +30,36 @@
     <t>Class</t>
   </si>
   <si>
+    <t>blues</t>
+  </si>
+  <si>
+    <t>classical</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>disco</t>
+  </si>
+  <si>
+    <t>hiphop</t>
+  </si>
+  <si>
+    <t>jazz</t>
+  </si>
+  <si>
+    <t>metal</t>
+  </si>
+  <si>
+    <t>pop</t>
+  </si>
+  <si>
+    <t>reggae</t>
+  </si>
+  <si>
+    <t>rock</t>
+  </si>
+  <si>
     <t>MSE</t>
   </si>
   <si>
@@ -45,6 +75,9 @@
     <t>F-measure</t>
   </si>
   <si>
+    <t>AUC</t>
+  </si>
+  <si>
     <t>Normalization function</t>
   </si>
   <si>
@@ -73,6 +106,75 @@
   </si>
   <si>
     <t>F-measure</t>
+  </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <t>Normalization function</t>
+  </si>
+  <si>
+    <t>zscore</t>
+  </si>
+  <si>
+    <t>norm</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Specificity</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>F-measure</t>
+  </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <t>Normalization function</t>
+  </si>
+  <si>
+    <t>zscore</t>
+  </si>
+  <si>
+    <t>norm</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Specificity</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>F-measure</t>
+  </si>
+  <si>
+    <t>AUC</t>
   </si>
 </sst>
 </file>
@@ -118,669 +220,763 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="true"/>
     <col min="2" max="2" width="5.5703125" customWidth="true"/>
-    <col min="3" max="3" width="14.7109375" customWidth="true"/>
+    <col min="3" max="3" width="6.7109375" customWidth="true"/>
     <col min="4" max="4" width="12.7109375" customWidth="true"/>
     <col min="5" max="5" width="12.7109375" customWidth="true"/>
     <col min="6" max="6" width="12.7109375" customWidth="true"/>
     <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="8" max="8" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>19</v>
+        <v>52</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B2" s="0"/>
       <c r="C2" s="0">
-        <v>11.628930817610064</v>
+        <v>82.599999999999994</v>
       </c>
       <c r="D2" s="0">
-        <v>0.65408805031446537</v>
+        <v>0.61623525760397269</v>
       </c>
       <c r="E2" s="0">
-        <v>0.59999999999999998</v>
+        <v>0.65509363295880141</v>
       </c>
       <c r="F2" s="0">
-        <v>0.65972222222222221</v>
+        <v>0.57730337078651672</v>
       </c>
       <c r="G2" s="0">
-        <v>0.77551020408163251</v>
+        <v>0.59992987147210619</v>
+      </c>
+      <c r="H2" s="0">
+        <v>0.61619850187265923</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B3" s="0"/>
       <c r="C3" s="0">
-        <v>0.056603773584905662</v>
+        <v>505.30000000000001</v>
       </c>
       <c r="D3" s="0">
-        <v>0.94339622641509435</v>
+        <v>0.84372749844816874</v>
       </c>
       <c r="E3" s="0">
-        <v>0.72727272727272729</v>
+        <v>0.72079900124843954</v>
       </c>
       <c r="F3" s="0">
-        <v>0.95945945945945943</v>
+        <v>0.96664169787765297</v>
       </c>
       <c r="G3" s="0">
-        <v>0.96928327645051193</v>
+        <v>0.86085212843258607</v>
+      </c>
+      <c r="H3" s="0">
+        <v>0.84372034956304609</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="0">
-        <v>15.10062893081761</v>
+        <v>726.70000000000005</v>
       </c>
       <c r="D4" s="0">
-        <v>0.66666666666666663</v>
+        <v>0.67017070142768476</v>
       </c>
       <c r="E4" s="0">
-        <v>0.8666666666666667</v>
+        <v>0.81315855181023711</v>
       </c>
       <c r="F4" s="0">
-        <v>0.64583333333333337</v>
+        <v>0.52714107365792751</v>
       </c>
       <c r="G4" s="0">
-        <v>0.77824267782426781</v>
+        <v>0.6131822616873065</v>
+      </c>
+      <c r="H4" s="0">
+        <v>0.67014981273408236</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B5" s="0"/>
       <c r="C5" s="0">
-        <v>21.157232704402517</v>
+        <v>685.79999999999995</v>
       </c>
       <c r="D5" s="0">
-        <v>0.57232704402515722</v>
+        <v>0.62625387957790191</v>
       </c>
       <c r="E5" s="0">
-        <v>0.73684210526315785</v>
+        <v>0.74406991260923838</v>
       </c>
       <c r="F5" s="0">
-        <v>0.55000000000000004</v>
+        <v>0.50846441947565535</v>
       </c>
       <c r="G5" s="0">
-        <v>0.69369369369369371</v>
+        <v>0.57050976903419537</v>
+      </c>
+      <c r="H5" s="0">
+        <v>0.62626716604244692</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0"/>
       <c r="C6" s="0">
-        <v>13.89308176100629</v>
+        <v>353.80000000000001</v>
       </c>
       <c r="D6" s="0">
-        <v>0.66666666666666663</v>
+        <v>0.71298882681564257</v>
       </c>
       <c r="E6" s="0">
-        <v>0.76923076923076927</v>
+        <v>0.79881398252184765</v>
       </c>
       <c r="F6" s="0">
-        <v>0.65753424657534243</v>
+        <v>0.62722846441947577</v>
       </c>
       <c r="G6" s="0">
-        <v>0.78367346938775506</v>
+        <v>0.68394005562413451</v>
+      </c>
+      <c r="H6" s="0">
+        <v>0.71302122347066166</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B7" s="0"/>
       <c r="C7" s="0">
-        <v>8.6100628930817606</v>
+        <v>182.59999999999999</v>
       </c>
       <c r="D7" s="0">
-        <v>0.74213836477987416</v>
+        <v>0.70444444444444454</v>
       </c>
       <c r="E7" s="0">
-        <v>0.8666666666666667</v>
+        <v>0.76444444444444437</v>
       </c>
       <c r="F7" s="0">
-        <v>0.72916666666666663</v>
+        <v>0.64444444444444449</v>
       </c>
       <c r="G7" s="0">
-        <v>0.83665338645418319</v>
+        <v>0.68414680438120201</v>
+      </c>
+      <c r="H7" s="0">
+        <v>0.70444444444444454</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B8" s="0"/>
       <c r="C8" s="0">
-        <v>0.62893081761006286</v>
+        <v>147.30000000000001</v>
       </c>
       <c r="D8" s="0">
-        <v>0.84905660377358494</v>
+        <v>0.79587523277467409</v>
       </c>
       <c r="E8" s="0">
-        <v>0.66666666666666663</v>
+        <v>0.74530586766541818</v>
       </c>
       <c r="F8" s="0">
-        <v>0.87681159420289856</v>
+        <v>0.84649188514357054</v>
       </c>
       <c r="G8" s="0">
-        <v>0.90977443609022557</v>
+        <v>0.80488203369522859</v>
+      </c>
+      <c r="H8" s="0">
+        <v>0.7958988764044943</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B9" s="0"/>
       <c r="C9" s="0">
-        <v>9.0817610062893088</v>
+        <v>792.20000000000005</v>
       </c>
       <c r="D9" s="0">
-        <v>0.69811320754716977</v>
+        <v>0.7352141527001862</v>
       </c>
       <c r="E9" s="0">
-        <v>0.77272727272727271</v>
+        <v>0.86887640449438219</v>
       </c>
       <c r="F9" s="0">
-        <v>0.68613138686131392</v>
+        <v>0.60181023720349569</v>
       </c>
       <c r="G9" s="0">
-        <v>0.79661016949152541</v>
+        <v>0.68960674502341024</v>
+      </c>
+      <c r="H9" s="0">
+        <v>0.73534332084893883</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B10" s="0"/>
       <c r="C10" s="0">
-        <v>24.962264150943398</v>
+        <v>1297.3</v>
       </c>
       <c r="D10" s="0">
-        <v>0.56603773584905659</v>
+        <v>0.70691185599006823</v>
       </c>
       <c r="E10" s="0">
-        <v>0.82352941176470584</v>
+        <v>0.90217228464419486</v>
       </c>
       <c r="F10" s="0">
-        <v>0.53521126760563376</v>
+        <v>0.51171036204744069</v>
       </c>
       <c r="G10" s="0">
-        <v>0.68778280542986425</v>
+        <v>0.63532076286790073</v>
+      </c>
+      <c r="H10" s="0">
+        <v>0.70694132334581783</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="0">
-        <v>35.377358490566039</v>
+        <v>977.39999999999998</v>
       </c>
       <c r="D11" s="0">
-        <v>0.50314465408805031</v>
+        <v>0.5917659838609558</v>
       </c>
       <c r="E11" s="0">
-        <v>0.81818181818181823</v>
+        <v>0.75413233458177276</v>
       </c>
       <c r="F11" s="0">
-        <v>0.47972972972972971</v>
+        <v>0.42945068664169794</v>
       </c>
       <c r="G11" s="0">
-        <v>0.64253393665158376</v>
+        <v>0.50764097115441231</v>
+      </c>
+      <c r="H11" s="0">
+        <v>0.59179151061173529</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B12" s="0"/>
       <c r="C12" s="0">
-        <v>3.6226415094339623</v>
+        <v>368.19999999999999</v>
       </c>
       <c r="D12" s="0">
-        <v>0.72327044025157228</v>
+        <v>0.63183426443202984</v>
       </c>
       <c r="E12" s="0">
-        <v>0.54545454545454541</v>
+        <v>0.64740324594257181</v>
       </c>
       <c r="F12" s="0">
-        <v>0.75182481751824815</v>
+        <v>0.61640449438202249</v>
       </c>
       <c r="G12" s="0">
-        <v>0.82399999999999995</v>
+        <v>0.61350043376448848</v>
+      </c>
+      <c r="H12" s="0">
+        <v>0.6319038701622971</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B13" s="0"/>
       <c r="C13" s="0">
-        <v>0.0062893081761006293</v>
+        <v>727.5</v>
       </c>
       <c r="D13" s="0">
-        <v>0.96855345911949686</v>
+        <v>0.832566728739913</v>
       </c>
       <c r="E13" s="0">
-        <v>0.75</v>
+        <v>0.68737827715355793</v>
       </c>
       <c r="F13" s="0">
-        <v>0.98639455782312924</v>
+        <v>0.97777777777777786</v>
       </c>
       <c r="G13" s="0">
-        <v>0.98305084745762705</v>
+        <v>0.85426162431072805</v>
+      </c>
+      <c r="H13" s="0">
+        <v>0.83257802746566778</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B14" s="0"/>
       <c r="C14" s="0">
-        <v>33.515723270440255</v>
+        <v>1799.5999999999999</v>
       </c>
       <c r="D14" s="0">
-        <v>0.45283018867924529</v>
+        <v>0.5817659838609559</v>
       </c>
       <c r="E14" s="0">
-        <v>0.53333333333333333</v>
+        <v>0.81205992509363278</v>
       </c>
       <c r="F14" s="0">
-        <v>0.44444444444444442</v>
+        <v>0.35151061173533077</v>
       </c>
       <c r="G14" s="0">
-        <v>0.59534883720930243</v>
+        <v>0.45400323607143012</v>
+      </c>
+      <c r="H14" s="0">
+        <v>0.58178526841448197</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B15" s="0"/>
       <c r="C15" s="0">
-        <v>36.327044025157235</v>
+        <v>2160.3000000000002</v>
       </c>
       <c r="D15" s="0">
-        <v>0.48427672955974843</v>
+        <v>0.64019242706393542</v>
       </c>
       <c r="E15" s="0">
-        <v>0.82352941176470584</v>
+        <v>0.89549313358302141</v>
       </c>
       <c r="F15" s="0">
-        <v>0.44366197183098594</v>
+        <v>0.38488139825218476</v>
       </c>
       <c r="G15" s="0">
-        <v>0.60576923076923073</v>
+        <v>0.51367730789464705</v>
+      </c>
+      <c r="H15" s="0">
+        <v>0.64018726591760289</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="0">
-        <v>46.515723270440255</v>
+        <v>1621.7</v>
       </c>
       <c r="D16" s="0">
-        <v>0.44654088050314467</v>
+        <v>0.63677219118559891</v>
       </c>
       <c r="E16" s="0">
-        <v>0.94117647058823528</v>
+        <v>0.85529338327091131</v>
       </c>
       <c r="F16" s="0">
-        <v>0.38732394366197181</v>
+        <v>0.41813982521847698</v>
       </c>
       <c r="G16" s="0">
-        <v>0.55555555555555547</v>
+        <v>0.53161617303060504</v>
+      </c>
+      <c r="H16" s="0">
+        <v>0.63671660424469423</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B17" s="0"/>
       <c r="C17" s="0">
-        <v>3.9308176100628929</v>
+        <v>578.29999999999995</v>
       </c>
       <c r="D17" s="0">
-        <v>0.74213836477987416</v>
+        <v>0.62499999999999989</v>
       </c>
       <c r="E17" s="0">
-        <v>0.57894736842105265</v>
+        <v>0.55333333333333323</v>
       </c>
       <c r="F17" s="0">
-        <v>0.76428571428571423</v>
+        <v>0.69666666666666655</v>
       </c>
       <c r="G17" s="0">
-        <v>0.83921568627450971</v>
+        <v>0.64212941141336333</v>
+      </c>
+      <c r="H17" s="0">
+        <v>0.62499999999999989</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B18" s="0"/>
       <c r="C18" s="0">
-        <v>0.62893081761006286</v>
+        <v>273.80000000000001</v>
       </c>
       <c r="D18" s="0">
-        <v>0.87421383647798745</v>
+        <v>0.81088454376163865</v>
       </c>
       <c r="E18" s="0">
-        <v>0.54545454545454541</v>
+        <v>0.77857677902621725</v>
       </c>
       <c r="F18" s="0">
-        <v>0.89864864864864868</v>
+        <v>0.84294631710362045</v>
       </c>
       <c r="G18" s="0">
-        <v>0.93006993006993011</v>
+        <v>0.81476642577620173</v>
+      </c>
+      <c r="H18" s="0">
+        <v>0.81076154806491874</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B19" s="0"/>
       <c r="C19" s="0">
-        <v>29.081761006289309</v>
+        <v>1586</v>
       </c>
       <c r="D19" s="0">
-        <v>0.57232704402515722</v>
+        <v>0.75641837368094345</v>
       </c>
       <c r="E19" s="0">
-        <v>1</v>
+        <v>0.97111111111111126</v>
       </c>
       <c r="F19" s="0">
-        <v>0.53103448275862064</v>
+        <v>0.54171036204744072</v>
       </c>
       <c r="G19" s="0">
-        <v>0.6936936936936936</v>
+        <v>0.68545323801730584</v>
+      </c>
+      <c r="H19" s="0">
+        <v>0.75641073657927582</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B20" s="0"/>
       <c r="C20" s="0">
-        <v>26.572327044025158</v>
+        <v>1696.2</v>
       </c>
       <c r="D20" s="0">
-        <v>0.55345911949685533</v>
+        <v>0.67856921166977047</v>
       </c>
       <c r="E20" s="0">
-        <v>0.83333333333333337</v>
+        <v>0.90548064918851456</v>
       </c>
       <c r="F20" s="0">
-        <v>0.51773049645390068</v>
+        <v>0.45171036204744064</v>
       </c>
       <c r="G20" s="0">
-        <v>0.67281105990783407</v>
+        <v>0.58291983017607241</v>
+      </c>
+      <c r="H20" s="0">
+        <v>0.67859550561797766</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B21" s="0"/>
       <c r="C21" s="0">
-        <v>4.2515723270440251</v>
+        <v>1617.9000000000001</v>
       </c>
       <c r="D21" s="0">
-        <v>0.76100628930817615</v>
+        <v>0.62121663563004337</v>
       </c>
       <c r="E21" s="0">
-        <v>0.5714285714285714</v>
+        <v>0.83298377028714099</v>
       </c>
       <c r="F21" s="0">
-        <v>0.77931034482758621</v>
+        <v>0.40931335830212234</v>
       </c>
       <c r="G21" s="0">
-        <v>0.85606060606060597</v>
+        <v>0.51442726989970444</v>
+      </c>
+      <c r="H21" s="0">
+        <v>0.62114856429463183</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B22" s="0"/>
       <c r="C22" s="0">
-        <v>9.0817610062893088</v>
+        <v>120.40000000000001</v>
       </c>
       <c r="D22" s="0">
-        <v>0.68553459119496851</v>
+        <v>0.66069522036002493</v>
       </c>
       <c r="E22" s="0">
-        <v>0.59999999999999998</v>
+        <v>0.60840199750312107</v>
       </c>
       <c r="F22" s="0">
-        <v>0.69444444444444442</v>
+        <v>0.71292134831460674</v>
       </c>
       <c r="G22" s="0">
-        <v>0.80000000000000004</v>
+        <v>0.67669264052968203</v>
+      </c>
+      <c r="H22" s="0">
+        <v>0.66066167290886391</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B23" s="0"/>
       <c r="C23" s="0">
-        <v>0.15723270440251572</v>
+        <v>645.70000000000005</v>
       </c>
       <c r="D23" s="0">
-        <v>0.9308176100628931</v>
+        <v>0.8270049658597145</v>
       </c>
       <c r="E23" s="0">
-        <v>0.55555555555555558</v>
+        <v>0.69064918851435686</v>
       </c>
       <c r="F23" s="0">
-        <v>0.97872340425531912</v>
+        <v>0.96327091136079912</v>
       </c>
       <c r="G23" s="0">
-        <v>0.96167247386759569</v>
+        <v>0.84802523925576012</v>
+      </c>
+      <c r="H23" s="0">
+        <v>0.82696004993757788</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B24" s="0"/>
       <c r="C24" s="0">
-        <v>13.308176100628931</v>
+        <v>1017.1</v>
       </c>
       <c r="D24" s="0">
-        <v>0.67295597484276726</v>
+        <v>0.66573246430788335</v>
       </c>
       <c r="E24" s="0">
-        <v>0.83333333333333337</v>
+        <v>0.83084893882646682</v>
       </c>
       <c r="F24" s="0">
-        <v>0.65248226950354615</v>
+        <v>0.50051186017478144</v>
       </c>
       <c r="G24" s="0">
-        <v>0.77966101694915257</v>
+        <v>0.59692127125349947</v>
+      </c>
+      <c r="H24" s="0">
+        <v>0.6656803995006243</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B25" s="0"/>
       <c r="C25" s="0">
-        <v>28.232704402515722</v>
+        <v>1422.0999999999999</v>
       </c>
       <c r="D25" s="0">
-        <v>0.54088050314465408</v>
+        <v>0.66903786468032289</v>
       </c>
       <c r="E25" s="0">
-        <v>0.72727272727272729</v>
+        <v>0.86981273408239712</v>
       </c>
       <c r="F25" s="0">
-        <v>0.52702702702702697</v>
+        <v>0.46825218476903874</v>
       </c>
       <c r="G25" s="0">
-        <v>0.6812227074235806</v>
+        <v>0.58168197820267742</v>
+      </c>
+      <c r="H25" s="0">
+        <v>0.6690324594257181</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B26" s="0"/>
       <c r="C26" s="0">
-        <v>12.735849056603774</v>
+        <v>1392.9000000000001</v>
       </c>
       <c r="D26" s="0">
-        <v>0.64150943396226412</v>
+        <v>0.6334667908131596</v>
       </c>
       <c r="E26" s="0">
-        <v>0.6470588235294118</v>
+        <v>0.83529338327091129</v>
       </c>
       <c r="F26" s="0">
-        <v>0.64084507042253525</v>
+        <v>0.43157303370786515</v>
       </c>
       <c r="G26" s="0">
-        <v>0.76150627615062771</v>
+        <v>0.53963251770635434</v>
+      </c>
+      <c r="H26" s="0">
+        <v>0.63343320848938833</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B27" s="0"/>
       <c r="C27" s="0">
-        <v>21.89308176100629</v>
+        <v>253.90000000000001</v>
       </c>
       <c r="D27" s="0">
-        <v>0.5911949685534591</v>
+        <v>0.64388888888888896</v>
       </c>
       <c r="E27" s="0">
-        <v>0.72727272727272729</v>
+        <v>0.72000000000000008</v>
       </c>
       <c r="F27" s="0">
-        <v>0.58108108108108103</v>
+        <v>0.56777777777777771</v>
       </c>
       <c r="G27" s="0">
-        <v>0.72573839662447259</v>
+        <v>0.61286463048284534</v>
+      </c>
+      <c r="H27" s="0">
+        <v>0.64388888888888896</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B28" s="0"/>
       <c r="C28" s="0">
-        <v>0.76100628930817615</v>
+        <v>480.69999999999999</v>
       </c>
       <c r="D28" s="0">
-        <v>0.91823899371069184</v>
+        <v>0.78028864059590297</v>
       </c>
       <c r="E28" s="0">
-        <v>0.90000000000000002</v>
+        <v>0.71290886392009989</v>
       </c>
       <c r="F28" s="0">
-        <v>0.91946308724832215</v>
+        <v>0.84757802746566779</v>
       </c>
       <c r="G28" s="0">
-        <v>0.95470383275261317</v>
+        <v>0.79363705439639998</v>
+      </c>
+      <c r="H28" s="0">
+        <v>0.78024344569288395</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B29" s="0"/>
       <c r="C29" s="0">
-        <v>20.433962264150942</v>
+        <v>1791.8</v>
       </c>
       <c r="D29" s="0">
-        <v>0.64150943396226412</v>
+        <v>0.73415890751086277</v>
       </c>
       <c r="E29" s="0">
-        <v>1</v>
+        <v>0.96888888888888902</v>
       </c>
       <c r="F29" s="0">
-        <v>0.59285714285714286</v>
+        <v>0.49941323345817723</v>
       </c>
       <c r="G29" s="0">
-        <v>0.74439461883408065</v>
+        <v>0.65212655389031948</v>
+      </c>
+      <c r="H29" s="0">
+        <v>0.73415106117353313</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B30" s="0"/>
       <c r="C30" s="0">
-        <v>27.39622641509434</v>
+        <v>1520</v>
       </c>
       <c r="D30" s="0">
-        <v>0.53459119496855345</v>
+        <v>0.62961824953445067</v>
       </c>
       <c r="E30" s="0">
-        <v>0.75</v>
+        <v>0.84217228464419469</v>
       </c>
       <c r="F30" s="0">
-        <v>0.51048951048951052</v>
+        <v>0.41716604244694133</v>
       </c>
       <c r="G30" s="0">
-        <v>0.66363636363636369</v>
+        <v>0.52802804121571678</v>
+      </c>
+      <c r="H30" s="0">
+        <v>0.62966916354556801</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B31" s="0"/>
       <c r="C31" s="0">
-        <v>42.289308176100626</v>
+        <v>1675</v>
       </c>
       <c r="D31" s="0">
-        <v>0.39622641509433965</v>
+        <v>0.56394165114835504</v>
       </c>
       <c r="E31" s="0">
-        <v>0.70833333333333337</v>
+        <v>0.7852559300873907</v>
       </c>
       <c r="F31" s="0">
-        <v>0.34074074074074073</v>
+        <v>0.34252184769038702</v>
       </c>
       <c r="G31" s="0">
-        <v>0.4893617021276595</v>
+        <v>0.43685430581011619</v>
+      </c>
+      <c r="H31" s="0">
+        <v>0.56388888888888888</v>
       </c>
     </row>
   </sheetData>

</xml_diff>